<commit_message>
more sword word 2.0
</commit_message>
<xml_diff>
--- a/sword-world-2/checklist.xlsx
+++ b/sword-world-2/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/sword-world-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Source/japanese-collectors-list/sword-world-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27388565-14C6-C746-A5C4-F164711B3CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EB7C84-A3DE-684C-9896-0049C9CFE3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{8CADE1BE-3ACC-0042-AA7A-DA7689A7BBAF}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="25480" windowHeight="15780" xr2:uid="{8CADE1BE-3ACC-0042-AA7A-DA7689A7BBAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="119">
   <si>
     <t>year</t>
   </si>
@@ -265,6 +265,132 @@
   </si>
   <si>
     <t>fortuna_code.jpg</t>
+  </si>
+  <si>
+    <t>faydan_museum.jpg</t>
+  </si>
+  <si>
+    <t>プレイヤーズ・ハンドブック フェイダン博物誌</t>
+  </si>
+  <si>
+    <t>Players Handbook Faydan Museum</t>
+  </si>
+  <si>
+    <t>salz_museum.jpg</t>
+  </si>
+  <si>
+    <t>プレイヤーズ・ハンドブック ザルツ博物誌</t>
+  </si>
+  <si>
+    <t>Players Handbook Salz Museum</t>
+  </si>
+  <si>
+    <t>プレイヤーズ・ハンドブック ユーレリア博物誌</t>
+  </si>
+  <si>
+    <t>Players Handbook Eurelia Natural History</t>
+  </si>
+  <si>
+    <t>eurelia.jpg</t>
+  </si>
+  <si>
+    <t>プレイヤーズ・ハンドブック ダグニア博物誌</t>
+  </si>
+  <si>
+    <t>Players Handbook Dagnia Museum</t>
+  </si>
+  <si>
+    <t>dagnia_museum.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">プレイヤーズ・ハンドブック ディルフラム博物誌 </t>
+  </si>
+  <si>
+    <t>Players Handbook Dilfram Museum</t>
+  </si>
+  <si>
+    <t>dilfram_museum.jpg</t>
+  </si>
+  <si>
+    <t>ソード・ワールド2.0 ツアー(1) ルーフェリア</t>
+  </si>
+  <si>
+    <t>Sword World 2.0 Tour 1: Luferia</t>
+  </si>
+  <si>
+    <t>luferia.jpg</t>
+  </si>
+  <si>
+    <t>ソード・ワールド2.0ツアー (2)　リオス</t>
+  </si>
+  <si>
+    <t>Sword World 2.0 Tour 2: Lios</t>
+  </si>
+  <si>
+    <t>lios.jpg</t>
+  </si>
+  <si>
+    <t>calzorals_magic_angel.jpg</t>
+  </si>
+  <si>
+    <t>バトルキャンペーンブックカルゾラルの魔動天使</t>
+  </si>
+  <si>
+    <t>Battle Campaign Book Calzoral's Magic Angel</t>
+  </si>
+  <si>
+    <t>バトルキャンペーンブック プロセルシア秘史 ―暁をうたう竜の姫</t>
+  </si>
+  <si>
+    <t>Battle Campaign Book Procercia Secret History-Dawn Princess</t>
+  </si>
+  <si>
+    <t>procercia_secret_history.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ストーリー&amp;データブックドラゴンレイド戦竜伝 </t>
+  </si>
+  <si>
+    <t>Story &amp; Data Book Dragon Raid Senryuden</t>
+  </si>
+  <si>
+    <t>dragon_raid_senryuden.jpg</t>
+  </si>
+  <si>
+    <t>グランドキャンペーン ドラゴンレイドビギンズ ‐白き竜の乙女‐</t>
+  </si>
+  <si>
+    <t>Grand Campaign Dragon Raid Begins-White Dragon Maiden-</t>
+  </si>
+  <si>
+    <t>white_dragon_maiden.jpg</t>
+  </si>
+  <si>
+    <t>ストーリー&amp;データブック ドラゴンレイド戦竜伝 (2)</t>
+  </si>
+  <si>
+    <t>Story &amp; Data Book Dragon Raid Senryuden (2)</t>
+  </si>
+  <si>
+    <t>dragon_raid_senryuden2.jpg</t>
+  </si>
+  <si>
+    <t>シナリオ集　挑戦! 魔剣が呼ぶ迷宮</t>
+  </si>
+  <si>
+    <t>Scenario Collection: Challenge! Labyrinth Called by the Magic Sword</t>
+  </si>
+  <si>
+    <t>シナリオ集(2) 風雲!歌声が響く都市</t>
+  </si>
+  <si>
+    <t>Scenario Collection (2) Fengyun! A City Where the Singing Voice Echoes</t>
+  </si>
+  <si>
+    <t>fengyun.jpg</t>
+  </si>
+  <si>
+    <t>labyrinth_magic_sword.jpg</t>
   </si>
 </sst>
 </file>
@@ -616,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281696FC-13B2-794A-AFD6-06FE8AA5DB5C}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1090,6 +1216,286 @@
         <v>46</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2012</v>
+      </c>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2012</v>
+      </c>
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2013</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2015</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2016</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2009</v>
+      </c>
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2010</v>
+      </c>
+      <c r="B30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2014</v>
+      </c>
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2015</v>
+      </c>
+      <c r="B32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2014</v>
+      </c>
+      <c r="B33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2014</v>
+      </c>
+      <c r="B34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2015</v>
+      </c>
+      <c r="B35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2008</v>
+      </c>
+      <c r="B36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>118</v>
+      </c>
+      <c r="F36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2008</v>
+      </c>
+      <c r="B37" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>